<commit_message>
Atualizando gráfico de GANTT
</commit_message>
<xml_diff>
--- a/Excel/Gráfico de GANTT.xlsx
+++ b/Excel/Gráfico de GANTT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\Documentos\Documentação\Gráficos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\Documentos\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA0ED1A-B223-443A-8B76-C53D75C2F97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01972784-F39F-4277-955D-492CB632E8CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="461" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,9 +129,6 @@
     <t>Documento de Layout de importação</t>
   </si>
   <si>
-    <t>Testes unitários (Alinhado com Yoshi</t>
-  </si>
-  <si>
     <t xml:space="preserve">Importação de dados do arquivo texto </t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>White Paper do projeto</t>
+  </si>
+  <si>
+    <t>Testes unitários (Alinhado com Yoshi)</t>
   </si>
 </sst>
 </file>
@@ -605,7 +605,21 @@
     <cellStyle name="Ruim" xfId="3" builtinId="27"/>
     <cellStyle name="Saída" xfId="5" builtinId="21"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="34">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1040,7 +1054,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.875</c:v>
+                  <c:v>0.93333333333333335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3083,27 +3097,27 @@
     <mergeCell ref="AJ1:AP1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B10 D3:G9 D10 G10">
-    <cfRule type="expression" dxfId="31" priority="5">
+    <cfRule type="expression" dxfId="33" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:BK10">
-    <cfRule type="expression" dxfId="30" priority="4">
+    <cfRule type="expression" dxfId="32" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C9">
-    <cfRule type="expression" dxfId="29" priority="3">
+    <cfRule type="expression" dxfId="31" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="28" priority="2">
+    <cfRule type="expression" dxfId="30" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:F10">
-    <cfRule type="expression" dxfId="27" priority="1">
+    <cfRule type="expression" dxfId="29" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3117,10 +3131,10 @@
   <dimension ref="A1:EQ37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="8" topLeftCell="BC30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="8" topLeftCell="BC24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3175,14 +3189,14 @@
       <c r="E5" s="34"/>
       <c r="F5" s="37">
         <f ca="1">TODAY()</f>
-        <v>44709</v>
+        <v>44711</v>
       </c>
       <c r="G5" s="37"/>
     </row>
     <row r="6" spans="1:147" s="2" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="27">
-        <f>(SUM(CÁLCULOS!A3:A22)/SUM('COM FÓRMULAS'!D9:D18))</f>
-        <v>0.875</v>
+        <f>(SUM(CÁLCULOS!A3:A22)/SUM('COM FÓRMULAS'!D9:D17))</f>
+        <v>0.93333333333333335</v>
       </c>
       <c r="D6" s="35" t="s">
         <v>7</v>
@@ -6236,7 +6250,7 @@
         <v>15</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D23" s="26">
         <v>1</v>
@@ -6719,7 +6733,7 @@
         <v>18</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26" s="26">
         <v>1</v>
@@ -7202,7 +7216,7 @@
         <v>21</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D29" s="26">
         <v>2</v>
@@ -7215,7 +7229,7 @@
         <v>44697</v>
       </c>
       <c r="G29" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H29" s="19"/>
       <c r="I29" s="19"/>
@@ -7537,7 +7551,7 @@
         <v>44700</v>
       </c>
       <c r="G31" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" s="19"/>
       <c r="I31" s="19"/>
@@ -7685,7 +7699,7 @@
         <v>24</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32" s="26">
         <v>2</v>
@@ -8010,18 +8024,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="EK7:EQ7"/>
-    <mergeCell ref="BE7:BK7"/>
-    <mergeCell ref="BS7:BY7"/>
-    <mergeCell ref="BZ7:CF7"/>
-    <mergeCell ref="CG7:CM7"/>
-    <mergeCell ref="CN7:CT7"/>
-    <mergeCell ref="CU7:DA7"/>
-    <mergeCell ref="DB7:DH7"/>
-    <mergeCell ref="DI7:DO7"/>
-    <mergeCell ref="DP7:DV7"/>
-    <mergeCell ref="DW7:EC7"/>
-    <mergeCell ref="ED7:EJ7"/>
     <mergeCell ref="AX7:BD7"/>
     <mergeCell ref="BL7:BR7"/>
     <mergeCell ref="A1:G2"/>
@@ -8038,39 +8040,51 @@
     <mergeCell ref="AC7:AI7"/>
     <mergeCell ref="AJ7:AP7"/>
     <mergeCell ref="AQ7:AW7"/>
+    <mergeCell ref="EK7:EQ7"/>
+    <mergeCell ref="BE7:BK7"/>
+    <mergeCell ref="BS7:BY7"/>
+    <mergeCell ref="BZ7:CF7"/>
+    <mergeCell ref="CG7:CM7"/>
+    <mergeCell ref="CN7:CT7"/>
+    <mergeCell ref="CU7:DA7"/>
+    <mergeCell ref="DB7:DH7"/>
+    <mergeCell ref="DI7:DO7"/>
+    <mergeCell ref="DP7:DV7"/>
+    <mergeCell ref="DW7:EC7"/>
+    <mergeCell ref="ED7:EJ7"/>
   </mergeCells>
   <conditionalFormatting sqref="B18:D19 B17 D17 B9:G10 B16:D16 E16:F33 B11:F15 B20:C20 B21:D32 G11:G33">
-    <cfRule type="expression" dxfId="26" priority="21">
+    <cfRule type="expression" dxfId="1" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:BD32 BL9:EQ32">
-    <cfRule type="expression" dxfId="25" priority="20">
+    <cfRule type="expression" dxfId="27" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:BD32 BL9:EQ32">
-    <cfRule type="expression" dxfId="24" priority="18">
+    <cfRule type="expression" dxfId="26" priority="18">
       <formula>AND(H$8&gt;=$E9,H$8&lt;=$F9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:BD32 BL9:EQ32">
-    <cfRule type="expression" dxfId="23" priority="19">
+    <cfRule type="expression" dxfId="25" priority="19">
       <formula>OR(WEEKDAY(H$8,2)=6,WEEKDAY(H$8,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE9:BK32">
-    <cfRule type="expression" dxfId="22" priority="16">
+    <cfRule type="expression" dxfId="24" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE9:BK32">
-    <cfRule type="expression" dxfId="21" priority="14">
+    <cfRule type="expression" dxfId="23" priority="14">
       <formula>AND(BE$8&gt;=$E9,BE$8&lt;=$F9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE9:BK32">
-    <cfRule type="expression" dxfId="20" priority="15">
+    <cfRule type="expression" dxfId="22" priority="15">
       <formula>OR(WEEKDAY(BE$8,2)=6,WEEKDAY(BE$8,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8089,47 +8103,47 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33:D33">
-    <cfRule type="expression" dxfId="19" priority="11">
+    <cfRule type="expression" dxfId="21" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:BD33 BL33:EQ33">
-    <cfRule type="expression" dxfId="18" priority="10">
+    <cfRule type="expression" dxfId="20" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:BD33 BL33:EQ33">
-    <cfRule type="expression" dxfId="17" priority="8">
+    <cfRule type="expression" dxfId="19" priority="8">
       <formula>AND(H$8&gt;=$E33,H$8&lt;=$F33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:BD33 BL33:EQ33">
-    <cfRule type="expression" dxfId="16" priority="9">
+    <cfRule type="expression" dxfId="18" priority="9">
       <formula>OR(WEEKDAY(H$8,2)=6,WEEKDAY(H$8,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE33:BK33">
-    <cfRule type="expression" dxfId="15" priority="6">
+    <cfRule type="expression" dxfId="17" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE33:BK33">
-    <cfRule type="expression" dxfId="14" priority="4">
+    <cfRule type="expression" dxfId="16" priority="4">
       <formula>AND(BE$8&gt;=$E33,BE$8&lt;=$F33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE33:BK33">
-    <cfRule type="expression" dxfId="13" priority="5">
+    <cfRule type="expression" dxfId="15" priority="5">
       <formula>OR(WEEKDAY(BE$8,2)=6,WEEKDAY(BE$8,2)=7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>